<commit_message>
add suavização de laplace
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2ºsemestre\Ciência dos dados\P2_tweets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Disciplinas\2° semestre\Ciência dos Dados\P2_tweets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{350D851C-BC45-4F57-A383-4B2B3AB8DF7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E7738B8-9EAC-4E37-8440-859934C0ADAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C3E0882-0726-4C5E-9EA2-2AAC294C2E75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{8A2B2A58-13B7-4CDF-A72E-F04AF7964E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+  <si>
+    <t>Teste</t>
+  </si>
   <si>
     <t>xiaomi é o celular que emite mais radiação só n perde p creu falando q n existe aquecimento global</t>
   </si>
@@ -721,8 +724,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -750,8 +761,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1065,17 +1077,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671F22CD-80FF-420D-8163-03C987F8E963}">
-  <dimension ref="A1:A200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0BBF2C-51FB-437C-B755-9F70BF44DB4D}">
+  <dimension ref="A1:A201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1991,12 +2006,12 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>128</v>
+        <v>183</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
@@ -2021,12 +2036,12 @@
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>105</v>
+        <v>188</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
@@ -2072,6 +2087,11 @@
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>